<commit_message>
Added Authentication and Authorization with config files.
</commit_message>
<xml_diff>
--- a/Schema Design/Schemas.xlsx
+++ b/Schema Design/Schemas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishi\OneDrive\Desktop\Node\Schema Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C0DDA6-5477-48E0-AA82-9E08380DEC02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3219D1-B27F-4394-A3D8-743A660AB6CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{63B837C1-41E2-47B2-B1B2-537C4BD5A316}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t>Students</t>
   </si>
@@ -193,13 +193,31 @@
   </si>
   <si>
     <t>SuperUser_ID</t>
+  </si>
+  <si>
+    <t>Authentication Endpoints</t>
+  </si>
+  <si>
+    <t>AuthParents</t>
+  </si>
+  <si>
+    <t>AuthDrivers</t>
+  </si>
+  <si>
+    <t>AuthSchoolAdmins</t>
+  </si>
+  <si>
+    <t>AuthSuperUsers</t>
+  </si>
+  <si>
+    <t>WorkFlow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,14 +227,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="7" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -295,15 +305,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -314,6 +324,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -369,6 +385,9 @@
             <a:gd name="adj" fmla="val 29070"/>
           </a:avLst>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -393,10 +412,14 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>               </a:t>
+            <a:t>                     </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>SuperUser</a:t>
           </a:r>
         </a:p>
@@ -436,6 +459,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -463,7 +489,11 @@
             <a:t>                  </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Admin</a:t>
           </a:r>
         </a:p>
@@ -559,6 +589,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -586,7 +619,11 @@
             <a:t>                  </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Parents</a:t>
           </a:r>
         </a:p>
@@ -626,6 +663,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -653,7 +693,11 @@
             <a:t>                  </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Students</a:t>
           </a:r>
         </a:p>
@@ -693,6 +737,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -717,10 +764,14 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>                  </a:t>
+            <a:t>                      </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Drivers</a:t>
           </a:r>
         </a:p>
@@ -760,6 +811,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -784,10 +838,14 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>                  </a:t>
+            <a:t>                      </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>School</a:t>
           </a:r>
         </a:p>
@@ -827,6 +885,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -854,7 +915,11 @@
             <a:t>                  </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Locations</a:t>
           </a:r>
         </a:p>
@@ -894,6 +959,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -918,10 +986,14 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>                  </a:t>
+            <a:t>               </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Buses</a:t>
           </a:r>
         </a:p>
@@ -961,6 +1033,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -985,10 +1060,14 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>                  </a:t>
+            <a:t>           </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Routes</a:t>
           </a:r>
         </a:p>
@@ -1420,6 +1499,9 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -1447,8 +1529,24 @@
             <a:t>           </a:t>
           </a:r>
           <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Daily</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Daily Attendance</a:t>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Attendance</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1811,10 +1909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CA4A4C-D98F-4F60-B24C-BB9338EBB26D}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1822,12 +1920,12 @@
     <col min="1" max="1" width="17.36328125" customWidth="1"/>
     <col min="2" max="2" width="17.453125" customWidth="1"/>
     <col min="3" max="3" width="18.08984375" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="17.1796875" customWidth="1"/>
-    <col min="8" max="8" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" customWidth="1"/>
     <col min="10" max="10" width="11.54296875" customWidth="1"/>
     <col min="11" max="11" width="14.36328125" customWidth="1"/>
   </cols>
@@ -1924,263 +2022,321 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="I17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="B19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" t="s">
-        <v>8</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="9"/>
+      <c r="D29" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="9"/>
+      <c r="D30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="7"/>
+      <c r="D31" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="11"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="7"/>
+      <c r="D32" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
@@ -2195,20 +2351,36 @@
       <c r="B34" s="7"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
     </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="13">
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A58:J58"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
@@ -2216,6 +2388,10 @@
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>